<commit_message>
Set up all dynamic references to LA name
</commit_message>
<xml_diff>
--- a/BSD Dummy Data - with add Q.xlsx
+++ b/BSD Dummy Data - with add Q.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\connachan.cara\Documents\building-standards-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D32C402-98CD-4E04-8C33-0AF6D60CE43C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BEEB11-626C-4328-BDE7-55BF77ED381A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="117">
   <si>
     <t>UserID</t>
   </si>
@@ -410,9 +410,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,13 +728,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CM10"/>
+  <dimension ref="A1:CM12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:91">
       <c r="A1" t="s">
@@ -3374,6 +3378,532 @@
         <v>75</v>
       </c>
       <c r="CM10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:91">
+      <c r="A11" s="2">
+        <v>1867584523</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" t="s">
+        <v>115</v>
+      </c>
+      <c r="I11" t="s">
+        <v>71</v>
+      </c>
+      <c r="J11" t="s">
+        <v>116</v>
+      </c>
+      <c r="K11" t="s">
+        <v>75</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11" t="s">
+        <v>75</v>
+      </c>
+      <c r="U11">
+        <v>32</v>
+      </c>
+      <c r="V11" t="s">
+        <v>75</v>
+      </c>
+      <c r="W11" t="s">
+        <v>75</v>
+      </c>
+      <c r="X11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI11">
+        <v>3</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM11">
+        <v>1</v>
+      </c>
+      <c r="AN11">
+        <v>4</v>
+      </c>
+      <c r="AO11">
+        <v>3</v>
+      </c>
+      <c r="AP11">
+        <v>1</v>
+      </c>
+      <c r="AQ11">
+        <v>5</v>
+      </c>
+      <c r="AR11">
+        <v>4</v>
+      </c>
+      <c r="AS11" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AU11" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV11" t="s">
+        <v>77</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AZ11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BB11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BE11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BG11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BH11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BI11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BJ11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BK11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BL11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BM11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BN11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BO11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BP11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BQ11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BR11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BS11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BT11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BU11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BV11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BW11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BX11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BZ11" t="s">
+        <v>75</v>
+      </c>
+      <c r="CA11" t="s">
+        <v>75</v>
+      </c>
+      <c r="CB11" t="s">
+        <v>75</v>
+      </c>
+      <c r="CC11" t="s">
+        <v>75</v>
+      </c>
+      <c r="CD11" t="s">
+        <v>75</v>
+      </c>
+      <c r="CE11" t="s">
+        <v>75</v>
+      </c>
+      <c r="CF11" t="s">
+        <v>75</v>
+      </c>
+      <c r="CG11" t="s">
+        <v>75</v>
+      </c>
+      <c r="CH11" t="s">
+        <v>75</v>
+      </c>
+      <c r="CI11" t="s">
+        <v>75</v>
+      </c>
+      <c r="CJ11" t="s">
+        <v>75</v>
+      </c>
+      <c r="CK11" t="s">
+        <v>75</v>
+      </c>
+      <c r="CL11" t="s">
+        <v>75</v>
+      </c>
+      <c r="CM11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:91">
+      <c r="A12" s="2">
+        <v>186757684</v>
+      </c>
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I12" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" t="s">
+        <v>90</v>
+      </c>
+      <c r="K12" t="s">
+        <v>75</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12" t="s">
+        <v>75</v>
+      </c>
+      <c r="U12">
+        <v>12</v>
+      </c>
+      <c r="V12" t="s">
+        <v>75</v>
+      </c>
+      <c r="W12" t="s">
+        <v>75</v>
+      </c>
+      <c r="X12" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AV12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AZ12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BB12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BE12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BG12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BH12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BI12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BJ12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BK12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BL12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BM12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BN12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BO12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BP12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BQ12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BR12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BS12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BT12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BU12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BV12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BW12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BX12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BZ12" t="s">
+        <v>75</v>
+      </c>
+      <c r="CA12" t="s">
+        <v>70</v>
+      </c>
+      <c r="CB12" t="s">
+        <v>76</v>
+      </c>
+      <c r="CC12">
+        <v>3</v>
+      </c>
+      <c r="CD12" t="s">
+        <v>76</v>
+      </c>
+      <c r="CE12">
+        <v>3</v>
+      </c>
+      <c r="CF12">
+        <v>3</v>
+      </c>
+      <c r="CG12">
+        <v>3</v>
+      </c>
+      <c r="CH12" t="s">
+        <v>75</v>
+      </c>
+      <c r="CI12">
+        <v>2</v>
+      </c>
+      <c r="CJ12" t="s">
+        <v>75</v>
+      </c>
+      <c r="CK12">
+        <v>4</v>
+      </c>
+      <c r="CL12" t="s">
+        <v>75</v>
+      </c>
+      <c r="CM12" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Recode all values for download data, fix financial years
</commit_message>
<xml_diff>
--- a/BSD Dummy Data - with add Q.xlsx
+++ b/BSD Dummy Data - with add Q.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\connachan.cara\Documents\building-standards-dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://impservihub-my.sharepoint.com/personal/nicholas_cassidy_improvementservice_org_uk/Documents/building-standards-dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BEEB11-626C-4328-BDE7-55BF77ED381A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{B7BEEB11-626C-4328-BDE7-55BF77ED381A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{264FE3AB-F55D-4B5C-866A-4A9A2F637523}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="119">
   <si>
     <t>UserID</t>
   </si>
@@ -314,9 +314,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>15:41:51.463</t>
-  </si>
-  <si>
     <t>15:42:09.420</t>
   </si>
   <si>
@@ -378,6 +375,15 @@
   </si>
   <si>
     <t>15:45:46.890</t>
+  </si>
+  <si>
+    <t>`2022-05-10</t>
+  </si>
+  <si>
+    <t>2022-05-10</t>
+  </si>
+  <si>
+    <t>2023-05-10</t>
   </si>
 </sst>
 </file>
@@ -410,10 +416,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,15 +738,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CM12"/>
+  <dimension ref="A1:CM13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:91">
@@ -2076,14 +2088,14 @@
       <c r="G6" t="s">
         <v>71</v>
       </c>
-      <c r="H6" t="s">
-        <v>95</v>
+      <c r="H6" s="4">
+        <v>0.65406785879629636</v>
       </c>
       <c r="I6" t="s">
         <v>71</v>
       </c>
       <c r="J6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K6" t="s">
         <v>91</v>
@@ -2331,52 +2343,52 @@
     </row>
     <row r="7" spans="1:91">
       <c r="A7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
         <v>97</v>
-      </c>
-      <c r="B7" t="s">
-        <v>98</v>
       </c>
       <c r="G7" t="s">
         <v>71</v>
       </c>
       <c r="H7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I7" t="s">
         <v>71</v>
       </c>
       <c r="J7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K7" t="s">
         <v>100</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7" t="s">
         <v>101</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7" t="s">
-        <v>102</v>
       </c>
       <c r="U7" t="s">
         <v>75</v>
@@ -2594,52 +2606,52 @@
     </row>
     <row r="8" spans="1:91">
       <c r="A8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" t="s">
         <v>103</v>
-      </c>
-      <c r="B8" t="s">
-        <v>104</v>
       </c>
       <c r="G8" t="s">
         <v>71</v>
       </c>
       <c r="H8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I8" t="s">
         <v>71</v>
       </c>
       <c r="J8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K8" t="s">
+        <v>100</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8" t="s">
         <v>101</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8" t="s">
-        <v>102</v>
       </c>
       <c r="U8" t="s">
         <v>75</v>
@@ -2857,52 +2869,52 @@
     </row>
     <row r="9" spans="1:91">
       <c r="A9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" t="s">
         <v>107</v>
-      </c>
-      <c r="B9" t="s">
-        <v>108</v>
       </c>
       <c r="G9" t="s">
         <v>71</v>
       </c>
       <c r="H9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I9" t="s">
         <v>71</v>
       </c>
       <c r="J9" t="s">
+        <v>109</v>
+      </c>
+      <c r="K9" t="s">
         <v>110</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9" t="s">
         <v>111</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9" t="s">
-        <v>112</v>
       </c>
       <c r="U9" t="s">
         <v>75</v>
@@ -3120,52 +3132,52 @@
     </row>
     <row r="10" spans="1:91">
       <c r="A10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
         <v>113</v>
       </c>
-      <c r="B10" t="s">
+      <c r="G10" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H10" t="s">
         <v>114</v>
       </c>
-      <c r="G10" t="s">
-        <v>71</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="I10" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J10" t="s">
         <v>115</v>
       </c>
-      <c r="I10" t="s">
-        <v>71</v>
-      </c>
-      <c r="J10" t="s">
-        <v>116</v>
-      </c>
       <c r="K10" t="s">
+        <v>110</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10" t="s">
         <v>111</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>1</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10" t="s">
-        <v>112</v>
       </c>
       <c r="U10" t="s">
         <v>75</v>
@@ -3392,13 +3404,13 @@
         <v>71</v>
       </c>
       <c r="H11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I11" t="s">
         <v>71</v>
       </c>
       <c r="J11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K11" t="s">
         <v>75</v>
@@ -3651,14 +3663,14 @@
       <c r="B12" s="2">
         <v>11</v>
       </c>
-      <c r="G12" t="s">
-        <v>71</v>
+      <c r="G12" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="H12" t="s">
         <v>89</v>
       </c>
-      <c r="I12" t="s">
-        <v>71</v>
+      <c r="I12" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="J12" t="s">
         <v>90</v>
@@ -3904,6 +3916,269 @@
         <v>75</v>
       </c>
       <c r="CM12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:91">
+      <c r="A13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="J13" t="s">
+        <v>109</v>
+      </c>
+      <c r="K13" t="s">
+        <v>110</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13" t="s">
+        <v>111</v>
+      </c>
+      <c r="U13" t="s">
+        <v>75</v>
+      </c>
+      <c r="V13" t="s">
+        <v>75</v>
+      </c>
+      <c r="W13" t="s">
+        <v>75</v>
+      </c>
+      <c r="X13" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM13">
+        <v>1</v>
+      </c>
+      <c r="AN13">
+        <v>1</v>
+      </c>
+      <c r="AO13">
+        <v>1</v>
+      </c>
+      <c r="AP13">
+        <v>1</v>
+      </c>
+      <c r="AQ13">
+        <v>1</v>
+      </c>
+      <c r="AR13">
+        <v>1</v>
+      </c>
+      <c r="AS13" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU13" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV13" t="s">
+        <v>70</v>
+      </c>
+      <c r="AW13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AZ13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BB13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BE13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BG13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BH13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BI13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BJ13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BK13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BL13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BM13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BN13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BO13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BP13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BQ13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BR13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BS13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BT13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BU13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BV13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BW13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BX13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BZ13" t="s">
+        <v>75</v>
+      </c>
+      <c r="CA13" t="s">
+        <v>75</v>
+      </c>
+      <c r="CB13" t="s">
+        <v>75</v>
+      </c>
+      <c r="CC13" t="s">
+        <v>75</v>
+      </c>
+      <c r="CD13" t="s">
+        <v>75</v>
+      </c>
+      <c r="CE13" t="s">
+        <v>75</v>
+      </c>
+      <c r="CF13" t="s">
+        <v>75</v>
+      </c>
+      <c r="CG13" t="s">
+        <v>75</v>
+      </c>
+      <c r="CH13" t="s">
+        <v>75</v>
+      </c>
+      <c r="CI13" t="s">
+        <v>75</v>
+      </c>
+      <c r="CJ13" t="s">
+        <v>75</v>
+      </c>
+      <c r="CK13" t="s">
+        <v>75</v>
+      </c>
+      <c r="CL13" t="s">
+        <v>75</v>
+      </c>
+      <c r="CM13" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add extra quarter data
</commit_message>
<xml_diff>
--- a/BSD Dummy Data - with add Q.xlsx
+++ b/BSD Dummy Data - with add Q.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://impservihub-my.sharepoint.com/personal/nicholas_cassidy_improvementservice_org_uk/Documents/building-standards-dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{B7BEEB11-626C-4328-BDE7-55BF77ED381A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{264FE3AB-F55D-4B5C-866A-4A9A2F637523}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{B7BEEB11-626C-4328-BDE7-55BF77ED381A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0525352F-E657-4B53-893F-08116E72BBD2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="119">
   <si>
     <t>UserID</t>
   </si>
@@ -383,7 +383,7 @@
     <t>2022-05-10</t>
   </si>
   <si>
-    <t>2023-05-10</t>
+    <t>2022-07-10</t>
   </si>
 </sst>
 </file>
@@ -738,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CM13"/>
+  <dimension ref="A1:CM14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3933,7 +3933,7 @@
         <v>108</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J13" t="s">
         <v>109</v>
@@ -4179,6 +4179,269 @@
         <v>75</v>
       </c>
       <c r="CM13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:91">
+      <c r="A14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" t="s">
+        <v>108</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J14" t="s">
+        <v>109</v>
+      </c>
+      <c r="K14" t="s">
+        <v>110</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14" t="s">
+        <v>111</v>
+      </c>
+      <c r="U14" t="s">
+        <v>75</v>
+      </c>
+      <c r="V14" t="s">
+        <v>75</v>
+      </c>
+      <c r="W14" t="s">
+        <v>75</v>
+      </c>
+      <c r="X14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM14">
+        <v>1</v>
+      </c>
+      <c r="AN14">
+        <v>1</v>
+      </c>
+      <c r="AO14">
+        <v>1</v>
+      </c>
+      <c r="AP14">
+        <v>1</v>
+      </c>
+      <c r="AQ14">
+        <v>1</v>
+      </c>
+      <c r="AR14">
+        <v>1</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV14" t="s">
+        <v>70</v>
+      </c>
+      <c r="AW14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AZ14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BB14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BE14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BG14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BH14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BI14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BJ14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BK14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BL14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BM14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BN14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BO14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BP14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BQ14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BR14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BS14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BT14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BU14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BV14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BW14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BX14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BZ14" t="s">
+        <v>75</v>
+      </c>
+      <c r="CA14" t="s">
+        <v>75</v>
+      </c>
+      <c r="CB14" t="s">
+        <v>75</v>
+      </c>
+      <c r="CC14" t="s">
+        <v>75</v>
+      </c>
+      <c r="CD14" t="s">
+        <v>75</v>
+      </c>
+      <c r="CE14" t="s">
+        <v>75</v>
+      </c>
+      <c r="CF14" t="s">
+        <v>75</v>
+      </c>
+      <c r="CG14" t="s">
+        <v>75</v>
+      </c>
+      <c r="CH14" t="s">
+        <v>75</v>
+      </c>
+      <c r="CI14" t="s">
+        <v>75</v>
+      </c>
+      <c r="CJ14" t="s">
+        <v>75</v>
+      </c>
+      <c r="CK14" t="s">
+        <v>75</v>
+      </c>
+      <c r="CL14" t="s">
+        <v>75</v>
+      </c>
+      <c r="CM14" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>